<commit_message>
New diff sized network test files
</commit_message>
<xml_diff>
--- a/test-files/demo-files/21-genes_31-edges_Schade-data_input.xlsx
+++ b/test-files/demo-files/21-genes_31-edges_Schade-data_input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr date1904="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28665" windowHeight="6510" tabRatio="679" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13760" tabRatio="679" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -18,12 +18,17 @@
     <sheet name="simulation_times" sheetId="14" r:id="rId9"/>
     <sheet name="network_b" sheetId="15" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="58">
   <si>
     <t>CIN5</t>
   </si>
@@ -622,19 +627,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -645,7 +650,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="13">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -656,7 +661,7 @@
         <v>5.6454699400469585E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="13">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -667,7 +672,7 @@
         <v>7.9330985366991902E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="13">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -678,7 +683,7 @@
         <v>1.9752304725644133E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="13">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -689,7 +694,7 @@
         <v>3.3795906765722E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="13">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -700,7 +705,7 @@
         <v>3.1020143371824505E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="13">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -711,7 +716,7 @@
         <v>0.14088825191106802</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="13">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -722,7 +727,7 @@
         <v>0.11154638144825144</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="13">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -733,7 +738,7 @@
         <v>0.1963159368179215</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="13">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -744,7 +749,7 @@
         <v>5.3889043874193077E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="13">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -755,7 +760,7 @@
         <v>0.12815831377911416</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="13">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -766,7 +771,7 @@
         <v>0.13211520958506387</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="13">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -777,7 +782,7 @@
         <v>4.3213186230593212E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="13">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -788,7 +793,7 @@
         <v>0.54876409005989424</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="13">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -799,7 +804,7 @@
         <v>0.14546368990806</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="13">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -810,7 +815,7 @@
         <v>6.6011579608223986E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="13">
       <c r="A17" s="5" t="s">
         <v>49</v>
       </c>
@@ -821,7 +826,7 @@
         <v>0.44288096825491846</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="13">
       <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
@@ -832,7 +837,7 @@
         <v>0.3788494714977898</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="13">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -843,7 +848,7 @@
         <v>4.4519366186329026E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="13">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
@@ -854,7 +859,7 @@
         <v>2.576736105652043E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="13">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
@@ -865,7 +870,7 @@
         <v>0.13010978300207396</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="13">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -878,8 +883,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -891,9 +901,9 @@
       <selection sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -904,7 +914,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -915,7 +925,7 @@
         <v>0.21400910999979947</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -926,7 +936,7 @@
         <v>-3.0097269423921845E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -937,7 +947,7 @@
         <v>-2.5854989373965038E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -948,7 +958,7 @@
         <v>7.7100242021748255E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -959,7 +969,7 @@
         <v>1.0092961615087226</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -970,7 +980,7 @@
         <v>0.12140532582048055</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -981,7 +991,7 @@
         <v>0.45591326049519942</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -992,7 +1002,7 @@
         <v>0.47055992894815318</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1003,7 +1013,7 @@
         <v>-6.4667318623537584E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1014,7 +1024,7 @@
         <v>-0.10300251273705402</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1025,7 +1035,7 @@
         <v>-0.17254649199890326</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1036,7 +1046,7 @@
         <v>-3.212494239192671E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1047,7 +1057,7 @@
         <v>-0.73701506582980847</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1058,7 +1068,7 @@
         <v>1.0800531504299524</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1069,7 +1079,7 @@
         <v>0.15846314839540446</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1080,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1091,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1102,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1113,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1124,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1137,6 +1147,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1144,19 +1159,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1167,7 +1182,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1178,7 +1193,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1189,7 +1204,7 @@
         <v>2.5672117798516494E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1200,7 +1215,7 @@
         <v>1.7328679513998631E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1211,7 +1226,7 @@
         <v>1.1002336199364211E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1233,7 +1248,7 @@
         <v>7.7016353395549478E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1244,7 +1259,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1255,7 +1270,7 @@
         <v>6.9314718055994526E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1266,7 +1281,7 @@
         <v>1.6503504299046318E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1277,7 +1292,7 @@
         <v>3.0136833937388925E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1288,7 +1303,7 @@
         <v>5.7762265046662105E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1299,7 +1314,7 @@
         <v>1.332975347230664E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1310,7 +1325,7 @@
         <v>1.2602676010180823E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1321,7 +1336,7 @@
         <v>3.0136833937388925E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1332,7 +1347,7 @@
         <v>3.3007008598092635E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
         <v>49</v>
       </c>
@@ -1343,7 +1358,7 @@
         <v>0.34657359027997264</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
@@ -1354,7 +1369,7 @@
         <v>0.23104906018664842</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -1365,7 +1380,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
@@ -1376,7 +1391,7 @@
         <v>7.453195489891885E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
@@ -1387,7 +1402,7 @@
         <v>4.9510512897138946E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -1401,8 +1416,13 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1410,18 +1430,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1441,7 +1461,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -1461,7 +1481,7 @@
         <v>0.48435089511121021</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="5" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -1481,7 +1501,7 @@
         <v>-0.81793317594908443</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="5" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
@@ -1501,7 +1521,7 @@
         <v>-0.75147912525362393</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -1521,7 +1541,7 @@
         <v>0.8561782188284095</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="5" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1541,7 +1561,7 @@
         <v>-0.37427042872419891</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="5" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -1561,7 +1581,7 @@
         <v>4.7013326873905102E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="5" customFormat="1">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -1581,7 +1601,7 @@
         <v>1.1248372482258766</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="5" customFormat="1">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1601,7 +1621,7 @@
         <v>-0.30259736113703295</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -1621,7 +1641,7 @@
         <v>0.55135867455041376</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="5" customFormat="1">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -1641,7 +1661,7 @@
         <v>5.8441255712988402E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="5" customFormat="1">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
@@ -1661,7 +1681,7 @@
         <v>0.34910882026688672</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="5" customFormat="1">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -1681,7 +1701,7 @@
         <v>-0.21167047056013749</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="5" customFormat="1">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1701,7 +1721,7 @@
         <v>0.70320378879765943</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="5" customFormat="1">
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
@@ -1721,7 +1741,7 @@
         <v>1.3499275795365722</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="5" customFormat="1">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
@@ -1741,7 +1761,7 @@
         <v>0.28201661662499822</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
         <v>49</v>
       </c>
@@ -1761,7 +1781,7 @@
         <v>-1.2538405721454773</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
@@ -1781,7 +1801,7 @@
         <v>-0.34874733011964443</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -1801,7 +1821,7 @@
         <v>-0.35846845614647627</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="5" customFormat="1">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
@@ -1821,7 +1841,7 @@
         <v>0.58491872133390754</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="5" customFormat="1">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
@@ -1841,7 +1861,7 @@
         <v>0.10759743563684412</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="5" customFormat="1">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -1863,7 +1883,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1875,14 +1900,14 @@
       <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1902,7 +1927,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -1922,7 +1947,7 @@
         <v>0.70113230605848431</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="5" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -1942,7 +1967,7 @@
         <v>0.64255017478057119</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="5" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
@@ -1962,7 +1987,7 @@
         <v>0.27838685574573035</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -1982,7 +2007,7 @@
         <v>0.63214516421357758</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="5" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -2002,7 +2027,7 @@
         <v>0.42823496437234221</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="5" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -2022,7 +2047,7 @@
         <v>4.8795433799243088E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="5" customFormat="1">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -2042,7 +2067,7 @@
         <v>0.49603588739778276</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="5" customFormat="1">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -2062,7 +2087,7 @@
         <v>0.87095586318119766</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -2082,7 +2107,7 @@
         <v>0.32190956976908647</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="5" customFormat="1">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -2102,7 +2127,7 @@
         <v>0.61484906015845053</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="5" customFormat="1">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
@@ -2122,7 +2147,7 @@
         <v>0.55944943488351928</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="5" customFormat="1">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -2142,7 +2167,7 @@
         <v>0.60909208857869224</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="5" customFormat="1">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -2162,7 +2187,7 @@
         <v>0.18767426433518369</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="5" customFormat="1">
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
@@ -2182,7 +2207,7 @@
         <v>1.0858535453491927</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="5" customFormat="1">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
@@ -2202,7 +2227,7 @@
         <v>0.31773877344830698</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
         <v>49</v>
       </c>
@@ -2222,7 +2247,7 @@
         <v>0.55774523004671794</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
@@ -2242,7 +2267,7 @@
         <v>1.28722744723447</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -2262,7 +2287,7 @@
         <v>0.83003274855249065</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="5" customFormat="1">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
@@ -2282,7 +2307,7 @@
         <v>0.29430825608901451</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="5" customFormat="1">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
@@ -2302,7 +2327,7 @@
         <v>0.14488756926375135</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="5" customFormat="1">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -2322,50 +2347,55 @@
         <v>0.80815140874532154</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" s="5" customFormat="1"/>
+    <row r="24" spans="1:6" s="5" customFormat="1"/>
+    <row r="25" spans="1:6" s="5" customFormat="1"/>
+    <row r="26" spans="1:6" s="5" customFormat="1"/>
+    <row r="27" spans="1:6" s="5" customFormat="1"/>
+    <row r="28" spans="1:6" s="5" customFormat="1"/>
+    <row r="29" spans="1:6" s="5" customFormat="1"/>
+    <row r="30" spans="1:6" s="5" customFormat="1"/>
+    <row r="31" spans="1:6" s="5" customFormat="1"/>
+    <row r="32" spans="1:6" s="5" customFormat="1"/>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.875" customWidth="1"/>
-    <col min="2" max="2" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.75" customWidth="1"/>
-    <col min="11" max="11" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -2433,7 +2463,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2501,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2569,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2637,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2705,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2773,12 +2803,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2802,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -2823,27 +2853,27 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <v>0</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2867,10 +2897,10 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -2897,21 +2927,21 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>0</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2935,10 +2965,10 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -2974,12 +3004,12 @@
         <v>0</v>
       </c>
       <c r="V9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="5" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3009,7 +3039,7 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -3045,9 +3075,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22">
       <c r="A11" s="5" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3062,7 +3092,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -3074,10 +3104,10 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -3113,12 +3143,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22">
       <c r="A12" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3130,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -3157,10 +3187,10 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -3178,15 +3208,15 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -3210,7 +3240,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3225,10 +3255,10 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -3246,12 +3276,12 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3278,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -3302,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -3314,18 +3344,18 @@
         <v>0</v>
       </c>
       <c r="V14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -3343,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -3355,22 +3385,22 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -3382,18 +3412,18 @@
         <v>0</v>
       </c>
       <c r="V15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="5" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -3411,7 +3441,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -3423,16 +3453,16 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -3453,9 +3483,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22">
       <c r="A17" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3521,9 +3551,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22">
       <c r="A18" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3589,9 +3619,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3657,9 +3687,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3725,9 +3755,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22">
       <c r="A21" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3790,82 +3820,19 @@
         <v>0</v>
       </c>
       <c r="V21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3877,25 +3844,25 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.875" customWidth="1"/>
-    <col min="2" max="2" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.625" customWidth="1"/>
-    <col min="11" max="11" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -3963,7 +3930,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -4031,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -4099,7 +4066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -4167,7 +4134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -4235,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -4303,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -4371,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -4439,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -4507,7 +4474,7 @@
         <v>-0.14286868649613396</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -4575,7 +4542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
@@ -4643,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -4711,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -4779,7 +4746,7 @@
         <v>0.5420485402062647</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -4847,7 +4814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
@@ -4915,7 +4882,7 @@
         <v>-0.1323464725248332</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -4983,7 +4950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22">
       <c r="A17" s="5" t="s">
         <v>43</v>
       </c>
@@ -5051,7 +5018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22">
       <c r="A18" s="5" t="s">
         <v>44</v>
       </c>
@@ -5119,7 +5086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22">
       <c r="A19" s="5" t="s">
         <v>45</v>
       </c>
@@ -5187,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22">
       <c r="A20" s="5" t="s">
         <v>46</v>
       </c>
@@ -5255,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22">
       <c r="A21" s="5" t="s">
         <v>47</v>
       </c>
@@ -5323,7 +5290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22">
       <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
@@ -5393,8 +5360,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5406,25 +5378,25 @@
       <selection sqref="A1:V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.875" customWidth="1"/>
-    <col min="2" max="2" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.75" customWidth="1"/>
-    <col min="11" max="11" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -5492,7 +5464,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -5560,7 +5532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -5628,7 +5600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -5696,7 +5668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -5764,7 +5736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -5832,7 +5804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -5900,7 +5872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -5968,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -6036,7 +6008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -6104,7 +6076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
@@ -6172,7 +6144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -6240,7 +6212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -6308,7 +6280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -6376,7 +6348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
@@ -6444,7 +6416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -6512,7 +6484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22">
       <c r="A17" s="5" t="s">
         <v>43</v>
       </c>
@@ -6580,7 +6552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22">
       <c r="A18" s="5" t="s">
         <v>44</v>
       </c>
@@ -6648,7 +6620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22">
       <c r="A19" s="5" t="s">
         <v>45</v>
       </c>
@@ -6716,7 +6688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22">
       <c r="A20" s="5" t="s">
         <v>46</v>
       </c>
@@ -6784,7 +6756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22">
       <c r="A21" s="5" t="s">
         <v>47</v>
       </c>
@@ -6852,7 +6824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22">
       <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
@@ -6922,8 +6894,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6935,12 +6912,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -6948,7 +6925,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -6956,7 +6933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -6964,7 +6941,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -6972,7 +6949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -6980,7 +6957,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -6988,7 +6965,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -6996,7 +6973,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -7008,6 +6985,11 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7019,9 +7001,9 @@
       <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -7067,5 +7049,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Undid demo sheet change
</commit_message>
<xml_diff>
--- a/test-files/demo-files/21-genes_31-edges_Schade-data_input.xlsx
+++ b/test-files/demo-files/21-genes_31-edges_Schade-data_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13760" tabRatio="679" activeTab="4"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="25120" windowHeight="13760" tabRatio="679" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="58">
   <si>
     <t>CIN5</t>
   </si>
@@ -2371,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2804,11 +2804,11 @@
       </c>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="5" t="s">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2832,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -2853,19 +2853,19 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <v>0</v>
       </c>
       <c r="U7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -2873,7 +2873,7 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2897,10 +2897,10 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -2927,21 +2927,21 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <v>0</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2965,10 +2965,10 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3004,12 +3004,12 @@
         <v>0</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="5" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3039,7 +3039,7 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3092,7 +3092,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -3104,10 +3104,10 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -3145,10 +3145,10 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3160,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -3187,10 +3187,10 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -3208,15 +3208,15 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -3240,7 +3240,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3255,10 +3255,10 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -3276,12 +3276,12 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3308,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -3344,18 +3344,18 @@
         <v>0</v>
       </c>
       <c r="V14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -3373,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -3385,22 +3385,22 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -3412,18 +3412,18 @@
         <v>0</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="5" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -3441,7 +3441,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -3453,16 +3453,16 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -3485,7 +3485,7 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3553,7 +3553,7 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3757,69 +3757,137 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
         <v>0</v>
       </c>
     </row>

</xml_diff>